<commit_message>
Adding list of all I:R regions in English name - Correcting Cappadocia Taurica
</commit_message>
<xml_diff>
--- a/Dictionary (stub).xlsx
+++ b/Dictionary (stub).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GABRIELE\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234E8D68-1877-435D-8C3B-D04CDF979464}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BE0C5E-CA80-4D97-95B7-D48E6E5DA913}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{9B5CDCCF-11B4-4D82-88C7-1DF7EDDF1AB3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6383" uniqueCount="3458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6798" uniqueCount="3859">
   <si>
     <t>English</t>
   </si>
@@ -10405,6 +10405,1209 @@
   </si>
   <si>
     <t>tripolitânia</t>
+  </si>
+  <si>
+    <t>Dacia</t>
+  </si>
+  <si>
+    <t>Albocensia</t>
+  </si>
+  <si>
+    <t>Apulensis</t>
+  </si>
+  <si>
+    <t>Costobocia</t>
+  </si>
+  <si>
+    <t>Cotinia</t>
+  </si>
+  <si>
+    <t>Iazygia</t>
+  </si>
+  <si>
+    <t>Porolissensis</t>
+  </si>
+  <si>
+    <t>Potulatensia</t>
+  </si>
+  <si>
+    <t>Dravida</t>
+  </si>
+  <si>
+    <t>Koda</t>
+  </si>
+  <si>
+    <t>Malayas</t>
+  </si>
+  <si>
+    <t>North Tambapamni</t>
+  </si>
+  <si>
+    <t>North Tondainadu</t>
+  </si>
+  <si>
+    <t>Pandiya</t>
+  </si>
+  <si>
+    <t>South Tambapamni</t>
+  </si>
+  <si>
+    <t>South Tondainadu</t>
+  </si>
+  <si>
+    <t>Sriparvata</t>
+  </si>
+  <si>
+    <t>Gallaecia</t>
+  </si>
+  <si>
+    <t>Asturia Meridionalis</t>
+  </si>
+  <si>
+    <t>Asturia Septentrionalis</t>
+  </si>
+  <si>
+    <t>Callaecia Meridionalis</t>
+  </si>
+  <si>
+    <t>Callaecia Septentrionalis</t>
+  </si>
+  <si>
+    <t>Cantabria</t>
+  </si>
+  <si>
+    <t>Vaccaeia Meridionalis</t>
+  </si>
+  <si>
+    <t>Vaccaeia Septentrionalis</t>
+  </si>
+  <si>
+    <t>Gandhara</t>
+  </si>
+  <si>
+    <t>Glausae</t>
+  </si>
+  <si>
+    <t>Kasmira</t>
+  </si>
+  <si>
+    <t>Madra</t>
+  </si>
+  <si>
+    <t>Panchanada</t>
+  </si>
+  <si>
+    <t>Sibae</t>
+  </si>
+  <si>
+    <t>Trigata</t>
+  </si>
+  <si>
+    <t>Gedrosia</t>
+  </si>
+  <si>
+    <t>East Omana</t>
+  </si>
+  <si>
+    <t>Gerrha</t>
+  </si>
+  <si>
+    <t>Parecania</t>
+  </si>
+  <si>
+    <t>Patalene</t>
+  </si>
+  <si>
+    <t>Rudiana</t>
+  </si>
+  <si>
+    <t>West Omana</t>
+  </si>
+  <si>
+    <t>Germania</t>
+  </si>
+  <si>
+    <t>Bructeria</t>
+  </si>
+  <si>
+    <t>Chamavia</t>
+  </si>
+  <si>
+    <t>Chasuaria</t>
+  </si>
+  <si>
+    <t>Chaucia</t>
+  </si>
+  <si>
+    <t>Frisia</t>
+  </si>
+  <si>
+    <t>Langobardia</t>
+  </si>
+  <si>
+    <t>Pharodenia</t>
+  </si>
+  <si>
+    <t>Semnonia</t>
+  </si>
+  <si>
+    <t>Sicambria</t>
+  </si>
+  <si>
+    <t>Germania Superior</t>
+  </si>
+  <si>
+    <t>Chattia</t>
+  </si>
+  <si>
+    <t>Latobrigia</t>
+  </si>
+  <si>
+    <t>Leucia</t>
+  </si>
+  <si>
+    <t>Mediomatricia</t>
+  </si>
+  <si>
+    <t>Tribocia</t>
+  </si>
+  <si>
+    <t>Vangionia</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Achaea</t>
+  </si>
+  <si>
+    <t>Aetolia</t>
+  </si>
+  <si>
+    <t>Arcadia</t>
+  </si>
+  <si>
+    <t>Attica</t>
+  </si>
+  <si>
+    <t>Boeotia</t>
+  </si>
+  <si>
+    <t>Crete</t>
+  </si>
+  <si>
+    <t>Cyclades</t>
+  </si>
+  <si>
+    <t>Epirus</t>
+  </si>
+  <si>
+    <t>Euboea</t>
+  </si>
+  <si>
+    <t>Laconia</t>
+  </si>
+  <si>
+    <t>Himalaya</t>
+  </si>
+  <si>
+    <t>Gilgit</t>
+  </si>
+  <si>
+    <t>North Tarim Basin</t>
+  </si>
+  <si>
+    <t>Pamir</t>
+  </si>
+  <si>
+    <t>Shule</t>
+  </si>
+  <si>
+    <t>South Tarim Basin</t>
+  </si>
+  <si>
+    <t>Suvarna Gotra</t>
+  </si>
+  <si>
+    <t>Zhangzhung</t>
+  </si>
+  <si>
+    <t>Illyria</t>
+  </si>
+  <si>
+    <t>Cataria</t>
+  </si>
+  <si>
+    <t>Dalmatia</t>
+  </si>
+  <si>
+    <t>Daorsia</t>
+  </si>
+  <si>
+    <t>Deuria</t>
+  </si>
+  <si>
+    <t>Histria</t>
+  </si>
+  <si>
+    <t>Illyria Graeca</t>
+  </si>
+  <si>
+    <t>Libernia</t>
+  </si>
+  <si>
+    <t>Italia</t>
+  </si>
+  <si>
+    <t>Ariminum</t>
+  </si>
+  <si>
+    <t>Aternum</t>
+  </si>
+  <si>
+    <t>Corsica</t>
+  </si>
+  <si>
+    <t>Dodecapolis</t>
+  </si>
+  <si>
+    <t>Latium</t>
+  </si>
+  <si>
+    <t>Picenum</t>
+  </si>
+  <si>
+    <t>Sardinia Australis</t>
+  </si>
+  <si>
+    <t>Sardinia Borealis</t>
+  </si>
+  <si>
+    <t>Tuscia</t>
+  </si>
+  <si>
+    <t>Karnata</t>
+  </si>
+  <si>
+    <t>Keralaputa</t>
+  </si>
+  <si>
+    <t>North Mahismandala</t>
+  </si>
+  <si>
+    <t>North Satiyaputa</t>
+  </si>
+  <si>
+    <t>South Mahismandala</t>
+  </si>
+  <si>
+    <t>South Satiyaputa</t>
+  </si>
+  <si>
+    <t>Vanavasi</t>
+  </si>
+  <si>
+    <t>Lower Egypt</t>
+  </si>
+  <si>
+    <t>Central Delta</t>
+  </si>
+  <si>
+    <t>Eastern Delta</t>
+  </si>
+  <si>
+    <t>Heptanomis</t>
+  </si>
+  <si>
+    <t>Memphis</t>
+  </si>
+  <si>
+    <t>Parva</t>
+  </si>
+  <si>
+    <t>Sinai</t>
+  </si>
+  <si>
+    <t>Western Delta</t>
+  </si>
+  <si>
+    <t>Lusitania</t>
+  </si>
+  <si>
+    <t>Aebocosia</t>
+  </si>
+  <si>
+    <t>Celticia Maoioris</t>
+  </si>
+  <si>
+    <t>Celticia Minoris</t>
+  </si>
+  <si>
+    <t>Lusitania Meridionalis</t>
+  </si>
+  <si>
+    <t>Lusitania Septentrionalis</t>
+  </si>
+  <si>
+    <t>Oppidania</t>
+  </si>
+  <si>
+    <t>Turdulia Occidentalis</t>
+  </si>
+  <si>
+    <t>Vettonia Meridionalis</t>
+  </si>
+  <si>
+    <t>Vettonia Septentrionalis</t>
+  </si>
+  <si>
+    <t>Macedonia</t>
+  </si>
+  <si>
+    <t>Chalkidiki</t>
+  </si>
+  <si>
+    <t>Dardania</t>
+  </si>
+  <si>
+    <t>Dindaria</t>
+  </si>
+  <si>
+    <t>Emathia</t>
+  </si>
+  <si>
+    <t>Paeonia</t>
+  </si>
+  <si>
+    <t>Pelagonia</t>
+  </si>
+  <si>
+    <t>Thessaly</t>
+  </si>
+  <si>
+    <t>Madhyadesa</t>
+  </si>
+  <si>
+    <t>Ahicchatra</t>
+  </si>
+  <si>
+    <t>East Cedi</t>
+  </si>
+  <si>
+    <t>Kasi</t>
+  </si>
+  <si>
+    <t>Kosala</t>
+  </si>
+  <si>
+    <t>Kuru</t>
+  </si>
+  <si>
+    <t>Malla</t>
+  </si>
+  <si>
+    <t>Pancala</t>
+  </si>
+  <si>
+    <t>Sthanisvara</t>
+  </si>
+  <si>
+    <t>West Cedi</t>
+  </si>
+  <si>
+    <t>Magna Graecia</t>
+  </si>
+  <si>
+    <t>Apulia</t>
+  </si>
+  <si>
+    <t>Bruttium</t>
+  </si>
+  <si>
+    <t>Campania</t>
+  </si>
+  <si>
+    <t>Lucania</t>
+  </si>
+  <si>
+    <t>Sicania</t>
+  </si>
+  <si>
+    <t>Siculia</t>
+  </si>
+  <si>
+    <t>Syracuse</t>
+  </si>
+  <si>
+    <t>Tarentum</t>
+  </si>
+  <si>
+    <t>Abhiria</t>
+  </si>
+  <si>
+    <t>Inner Saurashtra</t>
+  </si>
+  <si>
+    <t>Kaccha</t>
+  </si>
+  <si>
+    <t>Outer Saurashtra</t>
+  </si>
+  <si>
+    <t>Oxydracae</t>
+  </si>
+  <si>
+    <t>Pardene</t>
+  </si>
+  <si>
+    <t>Sauvira</t>
+  </si>
+  <si>
+    <t>Mauretania</t>
+  </si>
+  <si>
+    <t>Massaesylia</t>
+  </si>
+  <si>
+    <t>Metagonia</t>
+  </si>
+  <si>
+    <t>Rutubis</t>
+  </si>
+  <si>
+    <t>Tadla</t>
+  </si>
+  <si>
+    <t>Tingitania</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Amardioi</t>
+  </si>
+  <si>
+    <t>Choarene</t>
+  </si>
+  <si>
+    <t>Kadousioi</t>
+  </si>
+  <si>
+    <t>Kossioi</t>
+  </si>
+  <si>
+    <t>Media Atropatene</t>
+  </si>
+  <si>
+    <t>Media Choromithrene</t>
+  </si>
+  <si>
+    <t>Media Magna</t>
+  </si>
+  <si>
+    <t>Paraetacene</t>
+  </si>
+  <si>
+    <t>Apolloniatis</t>
+  </si>
+  <si>
+    <t>Aramaea</t>
+  </si>
+  <si>
+    <t>Babylonia</t>
+  </si>
+  <si>
+    <t>Chaldaea</t>
+  </si>
+  <si>
+    <t>Characene</t>
+  </si>
+  <si>
+    <t>Garamaea</t>
+  </si>
+  <si>
+    <t>Sittacene</t>
+  </si>
+  <si>
+    <t>Sumer</t>
+  </si>
+  <si>
+    <t>Moesia</t>
+  </si>
+  <si>
+    <t>Getia</t>
+  </si>
+  <si>
+    <t>Malvensis</t>
+  </si>
+  <si>
+    <t>Picensia</t>
+  </si>
+  <si>
+    <t>Roxolania</t>
+  </si>
+  <si>
+    <t>Saldensia</t>
+  </si>
+  <si>
+    <t>Scordiscia</t>
+  </si>
+  <si>
+    <t>Tricornensia</t>
+  </si>
+  <si>
+    <t>Nubia</t>
+  </si>
+  <si>
+    <t>Alana</t>
+  </si>
+  <si>
+    <t>Alut</t>
+  </si>
+  <si>
+    <t>Aswan</t>
+  </si>
+  <si>
+    <t>Meroe</t>
+  </si>
+  <si>
+    <t>Napata</t>
+  </si>
+  <si>
+    <t>North Nubia</t>
+  </si>
+  <si>
+    <t>South Nubia</t>
+  </si>
+  <si>
+    <t>Numidia</t>
+  </si>
+  <si>
+    <t>Aurasius</t>
+  </si>
+  <si>
+    <t>Cirtania</t>
+  </si>
+  <si>
+    <t>Gaetulia</t>
+  </si>
+  <si>
+    <t>Iolia</t>
+  </si>
+  <si>
+    <t>Machuria</t>
+  </si>
+  <si>
+    <t>Massylia</t>
+  </si>
+  <si>
+    <t>Sitifensia</t>
+  </si>
+  <si>
+    <t>Zaba</t>
+  </si>
+  <si>
+    <t>Palestine</t>
+  </si>
+  <si>
+    <t>Arabia Petrea</t>
+  </si>
+  <si>
+    <t>Decapolis</t>
+  </si>
+  <si>
+    <t>Galilee</t>
+  </si>
+  <si>
+    <t>Judea</t>
+  </si>
+  <si>
+    <t>Peraea</t>
+  </si>
+  <si>
+    <t>Philistia</t>
+  </si>
+  <si>
+    <t>Samaria</t>
+  </si>
+  <si>
+    <t>Pannonia</t>
+  </si>
+  <si>
+    <t>Carnuntia</t>
+  </si>
+  <si>
+    <t>Hercuniatia</t>
+  </si>
+  <si>
+    <t>Latobicia</t>
+  </si>
+  <si>
+    <t>Pannonia Prima</t>
+  </si>
+  <si>
+    <t>Pannonia Secunda</t>
+  </si>
+  <si>
+    <t>Quadia</t>
+  </si>
+  <si>
+    <t>Valeria</t>
+  </si>
+  <si>
+    <t>Varciania</t>
+  </si>
+  <si>
+    <t>Parthia</t>
+  </si>
+  <si>
+    <t>Comisene</t>
+  </si>
+  <si>
+    <t>Hyrcania</t>
+  </si>
+  <si>
+    <t>Parnia</t>
+  </si>
+  <si>
+    <t>Siracene</t>
+  </si>
+  <si>
+    <t>Tapuria</t>
+  </si>
+  <si>
+    <t>Traxiane</t>
+  </si>
+  <si>
+    <t>Persis</t>
+  </si>
+  <si>
+    <t>Mardiene</t>
+  </si>
+  <si>
+    <t>Media Felix</t>
+  </si>
+  <si>
+    <t>Susiana</t>
+  </si>
+  <si>
+    <t>Tabiene</t>
+  </si>
+  <si>
+    <t>Taocene</t>
+  </si>
+  <si>
+    <t>Utia</t>
+  </si>
+  <si>
+    <t>Phrygia</t>
+  </si>
+  <si>
+    <t>Isauria</t>
+  </si>
+  <si>
+    <t>Lycaonia</t>
+  </si>
+  <si>
+    <t>Phrygia Maioris</t>
+  </si>
+  <si>
+    <t>Phrygia Minoris</t>
+  </si>
+  <si>
+    <t>Phrygia Parorea</t>
+  </si>
+  <si>
+    <t>Phrygia Ripensis</t>
+  </si>
+  <si>
+    <t>Phrygia Ulterioris</t>
+  </si>
+  <si>
+    <t>Pracya</t>
+  </si>
+  <si>
+    <t>Anga</t>
+  </si>
+  <si>
+    <t>Kamarupa</t>
+  </si>
+  <si>
+    <t>Kamata</t>
+  </si>
+  <si>
+    <t>Magadha</t>
+  </si>
+  <si>
+    <t>Pundra</t>
+  </si>
+  <si>
+    <t>Samatata</t>
+  </si>
+  <si>
+    <t>Vanga</t>
+  </si>
+  <si>
+    <t>Vrji</t>
+  </si>
+  <si>
+    <t>Punt</t>
+  </si>
+  <si>
+    <t>Aksum</t>
+  </si>
+  <si>
+    <t>Atbaras</t>
+  </si>
+  <si>
+    <t>Mosylon</t>
+  </si>
+  <si>
+    <t>Ptolemais Epithera</t>
+  </si>
+  <si>
+    <t>Tana</t>
+  </si>
+  <si>
+    <t>Rhaetia</t>
+  </si>
+  <si>
+    <t>Alpes Carniae</t>
+  </si>
+  <si>
+    <t>Alpes Graiae</t>
+  </si>
+  <si>
+    <t>Alpes Raetiae</t>
+  </si>
+  <si>
+    <t>Breunia</t>
+  </si>
+  <si>
+    <t>Helvetia</t>
+  </si>
+  <si>
+    <t>Noricum</t>
+  </si>
+  <si>
+    <t>Verbigenia</t>
+  </si>
+  <si>
+    <t>Sarmatia Asiatica</t>
+  </si>
+  <si>
+    <t>Alania</t>
+  </si>
+  <si>
+    <t>Alania Orientalis</t>
+  </si>
+  <si>
+    <t>Borysthenia Maioris</t>
+  </si>
+  <si>
+    <t>Confluenta</t>
+  </si>
+  <si>
+    <t>Danaia</t>
+  </si>
+  <si>
+    <t>Danaia Superioris</t>
+  </si>
+  <si>
+    <t>Mantessa</t>
+  </si>
+  <si>
+    <t>Sarmatia Europea</t>
+  </si>
+  <si>
+    <t>Borysthenia</t>
+  </si>
+  <si>
+    <t>Clepia</t>
+  </si>
+  <si>
+    <t>Hypania</t>
+  </si>
+  <si>
+    <t>Hypania Minoris</t>
+  </si>
+  <si>
+    <t>Olbia</t>
+  </si>
+  <si>
+    <t>Sarmatia</t>
+  </si>
+  <si>
+    <t>Sarmatia Superioris</t>
+  </si>
+  <si>
+    <t>Transborysthenia</t>
+  </si>
+  <si>
+    <t>Transhypania</t>
+  </si>
+  <si>
+    <t>Scandia</t>
+  </si>
+  <si>
+    <t>Cimbrica</t>
+  </si>
+  <si>
+    <t>East Gothia</t>
+  </si>
+  <si>
+    <t>Herulia</t>
+  </si>
+  <si>
+    <t>Scandia Insula</t>
+  </si>
+  <si>
+    <t>Ultima Thule</t>
+  </si>
+  <si>
+    <t>West Gothia</t>
+  </si>
+  <si>
+    <t>Scythia</t>
+  </si>
+  <si>
+    <t>Atara</t>
+  </si>
+  <si>
+    <t>Chorasmia</t>
+  </si>
+  <si>
+    <t>Dahaea</t>
+  </si>
+  <si>
+    <t>Darn</t>
+  </si>
+  <si>
+    <t>Hyrcania Superioris</t>
+  </si>
+  <si>
+    <t>Scythia Ad Pontem</t>
+  </si>
+  <si>
+    <t>Scythia Magna</t>
+  </si>
+  <si>
+    <t>Scythia Ultima</t>
+  </si>
+  <si>
+    <t>Transhyrcania</t>
+  </si>
+  <si>
+    <t>Sogdiana</t>
+  </si>
+  <si>
+    <t>Chach</t>
+  </si>
+  <si>
+    <t>Chomaria</t>
+  </si>
+  <si>
+    <t>Ferghana</t>
+  </si>
+  <si>
+    <t>Jaxartia</t>
+  </si>
+  <si>
+    <t>Kyreschata</t>
+  </si>
+  <si>
+    <t>Talas</t>
+  </si>
+  <si>
+    <t>Syria</t>
+  </si>
+  <si>
+    <t>Apamene</t>
+  </si>
+  <si>
+    <t>Coele Syria</t>
+  </si>
+  <si>
+    <t>Cyrrhestica</t>
+  </si>
+  <si>
+    <t>North Phoenicia</t>
+  </si>
+  <si>
+    <t>Palmyrene</t>
+  </si>
+  <si>
+    <t>South Phoenicia</t>
+  </si>
+  <si>
+    <t>Tarraconensis</t>
+  </si>
+  <si>
+    <t>Autrigonia</t>
+  </si>
+  <si>
+    <t>Celtiberia Centralis</t>
+  </si>
+  <si>
+    <t>Celtiberia Septentrionalis</t>
+  </si>
+  <si>
+    <t>Cessetania</t>
+  </si>
+  <si>
+    <t>Ilercavonia</t>
+  </si>
+  <si>
+    <t>Ilergetia</t>
+  </si>
+  <si>
+    <t>Indicetia</t>
+  </si>
+  <si>
+    <t>Vardulia</t>
+  </si>
+  <si>
+    <t>Vasconia</t>
+  </si>
+  <si>
+    <t>Borysthenia Minoris</t>
+  </si>
+  <si>
+    <t>Bosporanum</t>
+  </si>
+  <si>
+    <t>Maeotia</t>
+  </si>
+  <si>
+    <t>Maeotia Minores</t>
+  </si>
+  <si>
+    <t>Sattara</t>
+  </si>
+  <si>
+    <t>Sindica</t>
+  </si>
+  <si>
+    <t>Tanaissa</t>
+  </si>
+  <si>
+    <t>Thrace</t>
+  </si>
+  <si>
+    <t>Crobyzoia</t>
+  </si>
+  <si>
+    <t>Europa</t>
+  </si>
+  <si>
+    <t>Haemimontus</t>
+  </si>
+  <si>
+    <t>Rhodope</t>
+  </si>
+  <si>
+    <t>Thracia</t>
+  </si>
+  <si>
+    <t>Triballia</t>
+  </si>
+  <si>
+    <t>Tibet</t>
+  </si>
+  <si>
+    <t>Chomolangma</t>
+  </si>
+  <si>
+    <t>Jangtang</t>
+  </si>
+  <si>
+    <t>Lhasa</t>
+  </si>
+  <si>
+    <t>Sumpa</t>
+  </si>
+  <si>
+    <t>Tsang</t>
+  </si>
+  <si>
+    <t>Yarlung</t>
+  </si>
+  <si>
+    <t>Transalpine Gaul</t>
+  </si>
+  <si>
+    <t>Allobrogia</t>
+  </si>
+  <si>
+    <t>Alpes Cottiae</t>
+  </si>
+  <si>
+    <t>Alpes Maritimae</t>
+  </si>
+  <si>
+    <t>Arvernia</t>
+  </si>
+  <si>
+    <t>Narbonensis</t>
+  </si>
+  <si>
+    <t>Vocontia</t>
+  </si>
+  <si>
+    <t>Volcatia</t>
+  </si>
+  <si>
+    <t>Upper Egypt</t>
+  </si>
+  <si>
+    <t>Asyut</t>
+  </si>
+  <si>
+    <t>Farfara</t>
+  </si>
+  <si>
+    <t>Kharga</t>
+  </si>
+  <si>
+    <t>Khargana</t>
+  </si>
+  <si>
+    <t>Luxor</t>
+  </si>
+  <si>
+    <t>Myos Hormos</t>
+  </si>
+  <si>
+    <t>Troglodytica</t>
+  </si>
+  <si>
+    <t>Venedia</t>
+  </si>
+  <si>
+    <t>Chrononia</t>
+  </si>
+  <si>
+    <t>Elysia</t>
+  </si>
+  <si>
+    <t>Helveconia</t>
+  </si>
+  <si>
+    <t>Lugia</t>
+  </si>
+  <si>
+    <t>Marsignia</t>
+  </si>
+  <si>
+    <t>Rugia</t>
+  </si>
+  <si>
+    <t>Sciria</t>
+  </si>
+  <si>
+    <t>Turuntia</t>
+  </si>
+  <si>
+    <t>Venedia Inferior</t>
+  </si>
+  <si>
+    <t>Vindhyaprstha</t>
+  </si>
+  <si>
+    <t>Andhra</t>
+  </si>
+  <si>
+    <t>Asmaka</t>
+  </si>
+  <si>
+    <t>Dakshina Kosala</t>
+  </si>
+  <si>
+    <t>Fanindrapura</t>
+  </si>
+  <si>
+    <t>Kalinga</t>
+  </si>
+  <si>
+    <t>Mahendragiri</t>
+  </si>
+  <si>
+    <t>Radha</t>
+  </si>
+  <si>
+    <t>Vidharba</t>
+  </si>
+  <si>
+    <t>Vistulia</t>
+  </si>
+  <si>
+    <t>Amadocia</t>
+  </si>
+  <si>
+    <t>Bassetia</t>
+  </si>
+  <si>
+    <t>Ciscarpathia</t>
+  </si>
+  <si>
+    <t>Ossioia</t>
+  </si>
+  <si>
+    <t>Subcarpathia</t>
+  </si>
+  <si>
+    <t>Vistulia Inferioris</t>
+  </si>
+  <si>
+    <t>Zargidava</t>
+  </si>
+  <si>
+    <t>Cappadocian Taurican</t>
+  </si>
+  <si>
+    <t>Cappadocie Taurique</t>
+  </si>
+  <si>
+    <t>cappadocio-taurique</t>
+  </si>
+  <si>
+    <t>Taurisch Kappadokien</t>
+  </si>
+  <si>
+    <t>kappadokisch-taurisch</t>
+  </si>
+  <si>
+    <t>Capadocia Táurica</t>
+  </si>
+  <si>
+    <t>capadocio-táurica</t>
+  </si>
+  <si>
+    <t>Таврикская Каппадокия</t>
+  </si>
+  <si>
+    <t>таврикско-каппадокийск</t>
+  </si>
+  <si>
+    <t>Tawrikska Kapadocja</t>
+  </si>
+  <si>
+    <t>tawriksko-kapadocijsk</t>
+  </si>
+  <si>
+    <t>가빠도기야다우리가</t>
+  </si>
+  <si>
+    <t>卡帕多细亚陶里卡</t>
+  </si>
+  <si>
+    <t>cappadocio-taurica</t>
+  </si>
+  <si>
+    <t>Capadócia Táurica</t>
+  </si>
+  <si>
+    <t>capadócio-táurica</t>
   </si>
 </sst>
 </file>
@@ -10769,11 +11972,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{377788CA-E10A-4734-92E1-DB72A5A421C7}">
-  <dimension ref="A1:AF219"/>
+  <dimension ref="A1:AF606"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A220" sqref="A220"/>
+      <pane ySplit="1" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C220" sqref="C220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -17037,10 +18240,10 @@
         <v>33</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>2685</v>
+        <v>3843</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>2696</v>
+        <v>3844</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>96</v>
@@ -17049,52 +18252,52 @@
         <v>392</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>2697</v>
+        <v>3845</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>2698</v>
+        <v>3846</v>
       </c>
       <c r="K71" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>2699</v>
+        <v>3847</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>2701</v>
+        <v>3848</v>
       </c>
       <c r="O71" s="2" t="s">
         <v>82</v>
       </c>
       <c r="P71" s="2" t="s">
-        <v>2702</v>
+        <v>3849</v>
       </c>
       <c r="Q71" s="2" t="s">
-        <v>2703</v>
+        <v>3850</v>
       </c>
       <c r="R71" s="2" t="s">
         <v>44</v>
       </c>
       <c r="S71" s="2" t="s">
-        <v>2704</v>
+        <v>3851</v>
       </c>
       <c r="T71" s="2" t="s">
-        <v>2705</v>
+        <v>3852</v>
       </c>
       <c r="U71" s="2" t="s">
         <v>47</v>
       </c>
       <c r="V71" s="2" t="s">
-        <v>2706</v>
+        <v>3853</v>
       </c>
       <c r="W71" s="2" t="s">
-        <v>2707</v>
+        <v>3854</v>
       </c>
       <c r="X71" s="2" t="s">
-        <v>2708</v>
+        <v>3855</v>
       </c>
       <c r="Y71" s="2" t="s">
-        <v>2700</v>
+        <v>2419</v>
       </c>
       <c r="Z71" s="2" t="s">
         <v>96</v>
@@ -17103,10 +18306,10 @@
         <v>450</v>
       </c>
       <c r="AB71" s="2" t="s">
-        <v>2597</v>
+        <v>3856</v>
       </c>
       <c r="AC71" s="2" t="s">
-        <v>2701</v>
+        <v>3857</v>
       </c>
       <c r="AD71" s="2" t="s">
         <v>221</v>
@@ -17115,7 +18318,7 @@
         <v>222</v>
       </c>
       <c r="AF71" s="2" t="s">
-        <v>2702</v>
+        <v>3858</v>
       </c>
     </row>
     <row r="72" spans="1:32" x14ac:dyDescent="0.25">
@@ -30366,6 +31569,2025 @@
       </c>
       <c r="AF219" s="2" t="s">
         <v>290</v>
+      </c>
+    </row>
+    <row r="220" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A220" s="2" t="s">
+        <v>3458</v>
+      </c>
+    </row>
+    <row r="221" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A221" s="2" t="s">
+        <v>3459</v>
+      </c>
+    </row>
+    <row r="222" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A222" s="2" t="s">
+        <v>3460</v>
+      </c>
+    </row>
+    <row r="223" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A223" s="2" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="224" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A224" s="2" t="s">
+        <v>3462</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="2" t="s">
+        <v>3463</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="2" t="s">
+        <v>3464</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="2" t="s">
+        <v>3465</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="2" t="s">
+        <v>3466</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="2" t="s">
+        <v>3467</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="2" t="s">
+        <v>3468</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="2" t="s">
+        <v>3469</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="2" t="s">
+        <v>3470</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="2" t="s">
+        <v>3471</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="2" t="s">
+        <v>3472</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="2" t="s">
+        <v>3473</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="2" t="s">
+        <v>3474</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="2" t="s">
+        <v>3475</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="2" t="s">
+        <v>3476</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="2" t="s">
+        <v>3477</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="2" t="s">
+        <v>3478</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="2" t="s">
+        <v>3479</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="2" t="s">
+        <v>3480</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" s="2" t="s">
+        <v>3481</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" s="2" t="s">
+        <v>3482</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" s="2" t="s">
+        <v>3483</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" s="2" t="s">
+        <v>3484</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" s="2" t="s">
+        <v>3485</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" s="2" t="s">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" s="2" t="s">
+        <v>3487</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" s="2" t="s">
+        <v>3488</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" s="2" t="s">
+        <v>3489</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" s="2" t="s">
+        <v>3490</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" s="2" t="s">
+        <v>3491</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" s="2" t="s">
+        <v>3492</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" s="2" t="s">
+        <v>3493</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" s="2" t="s">
+        <v>3494</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" s="2" t="s">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" s="2" t="s">
+        <v>3496</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="2" t="s">
+        <v>3497</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" s="2" t="s">
+        <v>3498</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" s="2" t="s">
+        <v>3499</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" s="2" t="s">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" s="2" t="s">
+        <v>3501</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" s="2" t="s">
+        <v>3502</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" s="2" t="s">
+        <v>3503</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" s="2" t="s">
+        <v>3504</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" s="2" t="s">
+        <v>3505</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" s="2" t="s">
+        <v>3506</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" s="2" t="s">
+        <v>3507</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" s="2" t="s">
+        <v>3508</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" s="2" t="s">
+        <v>3509</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" s="2" t="s">
+        <v>3510</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" s="2" t="s">
+        <v>3511</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" s="2" t="s">
+        <v>3512</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" s="2" t="s">
+        <v>3513</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" s="2" t="s">
+        <v>3514</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" s="2" t="s">
+        <v>3515</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" s="2" t="s">
+        <v>3516</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" s="2" t="s">
+        <v>3517</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" s="2" t="s">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" s="2" t="s">
+        <v>3519</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" s="2" t="s">
+        <v>3520</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" s="2" t="s">
+        <v>3521</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" s="2" t="s">
+        <v>3522</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" s="2" t="s">
+        <v>3523</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" s="2" t="s">
+        <v>3524</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" s="2" t="s">
+        <v>3525</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" s="2" t="s">
+        <v>3526</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" s="2" t="s">
+        <v>3527</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" s="2" t="s">
+        <v>3528</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" s="2" t="s">
+        <v>3529</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" s="2" t="s">
+        <v>3530</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" s="2" t="s">
+        <v>3531</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" s="2" t="s">
+        <v>3532</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" s="2" t="s">
+        <v>3533</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" s="2" t="s">
+        <v>3534</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" s="2" t="s">
+        <v>3535</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" s="2" t="s">
+        <v>3536</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" s="2" t="s">
+        <v>3537</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" s="2" t="s">
+        <v>3538</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" s="2" t="s">
+        <v>3539</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" s="2" t="s">
+        <v>3540</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" s="2" t="s">
+        <v>3541</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" s="2" t="s">
+        <v>3542</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" s="2" t="s">
+        <v>3543</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" s="2" t="s">
+        <v>3544</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" s="2" t="s">
+        <v>3545</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" s="2" t="s">
+        <v>3546</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" s="2" t="s">
+        <v>3547</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" s="2" t="s">
+        <v>3548</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" s="2" t="s">
+        <v>3549</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" s="2" t="s">
+        <v>3550</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" s="2" t="s">
+        <v>3551</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314" s="2" t="s">
+        <v>3552</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315" s="2" t="s">
+        <v>3553</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316" s="2" t="s">
+        <v>3554</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A317" s="2" t="s">
+        <v>3555</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318" s="2" t="s">
+        <v>3556</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319" s="2" t="s">
+        <v>3557</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320" s="2" t="s">
+        <v>3558</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321" s="2" t="s">
+        <v>3559</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322" s="2" t="s">
+        <v>3560</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A323" s="2" t="s">
+        <v>3561</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324" s="2" t="s">
+        <v>3562</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325" s="2" t="s">
+        <v>3563</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326" s="2" t="s">
+        <v>3564</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327" s="2" t="s">
+        <v>3565</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328" s="2" t="s">
+        <v>3566</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A329" s="2" t="s">
+        <v>3567</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330" s="2" t="s">
+        <v>3568</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331" s="2" t="s">
+        <v>3569</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332" s="2" t="s">
+        <v>3570</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A333" s="2" t="s">
+        <v>3571</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334" s="2" t="s">
+        <v>3572</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A335" s="2" t="s">
+        <v>3573</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336" s="2" t="s">
+        <v>3574</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" s="2" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338" s="2" t="s">
+        <v>3576</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339" s="2" t="s">
+        <v>3577</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A340" s="2" t="s">
+        <v>3578</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A341" s="2" t="s">
+        <v>3579</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A342" s="2" t="s">
+        <v>3580</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A343" s="2" t="s">
+        <v>3581</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A344" s="2" t="s">
+        <v>3582</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A345" s="2" t="s">
+        <v>3583</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A346" s="2" t="s">
+        <v>3584</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A347" s="2" t="s">
+        <v>3585</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A348" s="2" t="s">
+        <v>3586</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349" s="2" t="s">
+        <v>3587</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A350" s="2" t="s">
+        <v>3588</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A351" s="2" t="s">
+        <v>3589</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352" s="2" t="s">
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353" s="2" t="s">
+        <v>3591</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A354" s="2" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355" s="2" t="s">
+        <v>3593</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356" s="2" t="s">
+        <v>3594</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357" s="2" t="s">
+        <v>3595</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358" s="2" t="s">
+        <v>3596</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359" s="2" t="s">
+        <v>3597</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" s="2" t="s">
+        <v>3598</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" s="2" t="s">
+        <v>3599</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" s="2" t="s">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363" s="2" t="s">
+        <v>3601</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" s="2" t="s">
+        <v>3602</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" s="2" t="s">
+        <v>3603</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" s="2" t="s">
+        <v>3604</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" s="2" t="s">
+        <v>3605</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" s="2" t="s">
+        <v>3606</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" s="2" t="s">
+        <v>3607</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" s="2" t="s">
+        <v>3608</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" s="2" t="s">
+        <v>3609</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" s="2" t="s">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" s="2" t="s">
+        <v>3611</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" s="2" t="s">
+        <v>3612</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" s="2" t="s">
+        <v>3613</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" s="2" t="s">
+        <v>3614</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" s="2" t="s">
+        <v>3615</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" s="2" t="s">
+        <v>3616</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" s="2" t="s">
+        <v>3617</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" s="2" t="s">
+        <v>3618</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" s="2" t="s">
+        <v>3619</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" s="2" t="s">
+        <v>3620</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" s="2" t="s">
+        <v>3621</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" s="2" t="s">
+        <v>3622</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" s="2" t="s">
+        <v>3623</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" s="2" t="s">
+        <v>3624</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" s="2" t="s">
+        <v>3625</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" s="2" t="s">
+        <v>3626</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" s="2" t="s">
+        <v>3627</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" s="2" t="s">
+        <v>3628</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" s="2" t="s">
+        <v>3629</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392" s="2" t="s">
+        <v>3630</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393" s="2" t="s">
+        <v>3631</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394" s="2" t="s">
+        <v>3632</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395" s="2" t="s">
+        <v>3633</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A396" s="2" t="s">
+        <v>3634</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397" s="2" t="s">
+        <v>3635</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398" s="2" t="s">
+        <v>3636</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A399" s="2" t="s">
+        <v>3637</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400" s="2" t="s">
+        <v>3638</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401" s="2" t="s">
+        <v>3639</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402" s="2" t="s">
+        <v>3640</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403" s="2" t="s">
+        <v>3641</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" s="2" t="s">
+        <v>3642</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" s="2" t="s">
+        <v>3643</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" s="2" t="s">
+        <v>3644</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" s="2" t="s">
+        <v>3645</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" s="2" t="s">
+        <v>3646</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" s="2" t="s">
+        <v>3647</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" s="2" t="s">
+        <v>3648</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" s="2" t="s">
+        <v>3649</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" s="2" t="s">
+        <v>3650</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" s="2" t="s">
+        <v>3651</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" s="2" t="s">
+        <v>3652</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" s="2" t="s">
+        <v>3653</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" s="2" t="s">
+        <v>3654</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" s="2" t="s">
+        <v>3655</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" s="2" t="s">
+        <v>3656</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" s="2" t="s">
+        <v>3657</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" s="2" t="s">
+        <v>3658</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" s="2" t="s">
+        <v>3659</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" s="2" t="s">
+        <v>3660</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" s="2" t="s">
+        <v>3661</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" s="2" t="s">
+        <v>3662</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" s="2" t="s">
+        <v>3663</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" s="2" t="s">
+        <v>3664</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" s="2" t="s">
+        <v>3665</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" s="2" t="s">
+        <v>3666</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429" s="2" t="s">
+        <v>3667</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" s="2" t="s">
+        <v>3668</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" s="2" t="s">
+        <v>3669</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" s="2" t="s">
+        <v>3670</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433" s="2" t="s">
+        <v>3671</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A434" s="2" t="s">
+        <v>3672</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A435" s="2" t="s">
+        <v>3673</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436" s="2" t="s">
+        <v>3674</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A437" s="2" t="s">
+        <v>3675</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A438" s="2" t="s">
+        <v>3676</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A439" s="2" t="s">
+        <v>3677</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440" s="2" t="s">
+        <v>3678</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441" s="2" t="s">
+        <v>3679</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442" s="2" t="s">
+        <v>3680</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443" s="2" t="s">
+        <v>3681</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" s="2" t="s">
+        <v>3682</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" s="2" t="s">
+        <v>3683</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" s="2" t="s">
+        <v>3684</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" s="2" t="s">
+        <v>3685</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448" s="2" t="s">
+        <v>3686</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" s="2" t="s">
+        <v>3687</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" s="2" t="s">
+        <v>3688</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451" s="2" t="s">
+        <v>3689</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452" s="2" t="s">
+        <v>3690</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A453" s="2" t="s">
+        <v>3691</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A454" s="2" t="s">
+        <v>3692</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A455" s="2" t="s">
+        <v>3693</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A456" s="2" t="s">
+        <v>3694</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A457" s="2" t="s">
+        <v>3695</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A458" s="2" t="s">
+        <v>3696</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A459" s="2" t="s">
+        <v>3697</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A460" s="2" t="s">
+        <v>3698</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A461" s="2" t="s">
+        <v>3699</v>
+      </c>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A462" s="2" t="s">
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A463" s="2" t="s">
+        <v>3701</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A464" s="2" t="s">
+        <v>3702</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465" s="2" t="s">
+        <v>3703</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A466" s="2" t="s">
+        <v>3704</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467" s="2" t="s">
+        <v>3705</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468" s="2" t="s">
+        <v>3706</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469" s="2" t="s">
+        <v>3707</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470" s="2" t="s">
+        <v>3708</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471" s="2" t="s">
+        <v>3709</v>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A472" s="2" t="s">
+        <v>3710</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" s="2" t="s">
+        <v>3711</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474" s="2" t="s">
+        <v>3712</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" s="2" t="s">
+        <v>3713</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" s="2" t="s">
+        <v>3714</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" s="2" t="s">
+        <v>3715</v>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" s="2" t="s">
+        <v>3716</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479" s="2" t="s">
+        <v>3717</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480" s="2" t="s">
+        <v>3718</v>
+      </c>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" s="2" t="s">
+        <v>3719</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A482" s="2" t="s">
+        <v>3720</v>
+      </c>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A483" s="2" t="s">
+        <v>3721</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A484" s="2" t="s">
+        <v>3722</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A485" s="2" t="s">
+        <v>3723</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A486" s="2" t="s">
+        <v>3724</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A487" s="2" t="s">
+        <v>3725</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A488" s="2" t="s">
+        <v>3726</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A489" s="2" t="s">
+        <v>3727</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A490" s="2" t="s">
+        <v>3728</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A491" s="2" t="s">
+        <v>3729</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A492" s="2" t="s">
+        <v>3730</v>
+      </c>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A493" s="2" t="s">
+        <v>3731</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A494" s="2" t="s">
+        <v>3732</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A495" s="2" t="s">
+        <v>3733</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A496" s="2" t="s">
+        <v>3734</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A497" s="2" t="s">
+        <v>3735</v>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A498" s="2" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A499" s="2" t="s">
+        <v>3737</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A500" s="2" t="s">
+        <v>3738</v>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A501" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A502" s="2" t="s">
+        <v>3739</v>
+      </c>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A503" s="2" t="s">
+        <v>3740</v>
+      </c>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A504" s="2" t="s">
+        <v>3741</v>
+      </c>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A505" s="2" t="s">
+        <v>3742</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A506" s="2" t="s">
+        <v>3743</v>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A507" s="2" t="s">
+        <v>3744</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A508" s="2" t="s">
+        <v>3745</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A509" s="2" t="s">
+        <v>3746</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A510" s="2" t="s">
+        <v>3747</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A511" s="2" t="s">
+        <v>3748</v>
+      </c>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A512" s="2" t="s">
+        <v>3749</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A513" s="2" t="s">
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A514" s="2" t="s">
+        <v>3751</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A515" s="2" t="s">
+        <v>3752</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A516" s="2" t="s">
+        <v>3753</v>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A517" s="2" t="s">
+        <v>3754</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A518" s="2" t="s">
+        <v>3755</v>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A519" s="2" t="s">
+        <v>3756</v>
+      </c>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A520" s="2" t="s">
+        <v>3757</v>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A521" s="2" t="s">
+        <v>3758</v>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A522" s="2" t="s">
+        <v>3759</v>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A523" s="2" t="s">
+        <v>3760</v>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A524" s="2" t="s">
+        <v>3761</v>
+      </c>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A525" s="2" t="s">
+        <v>3762</v>
+      </c>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A526" s="2" t="s">
+        <v>3763</v>
+      </c>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A527" s="2" t="s">
+        <v>3764</v>
+      </c>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A528" s="2" t="s">
+        <v>3765</v>
+      </c>
+    </row>
+    <row r="529" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A529" s="2" t="s">
+        <v>3766</v>
+      </c>
+    </row>
+    <row r="530" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A530" s="2" t="s">
+        <v>3767</v>
+      </c>
+    </row>
+    <row r="531" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A531" s="2" t="s">
+        <v>3768</v>
+      </c>
+    </row>
+    <row r="532" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A532" s="2" t="s">
+        <v>3769</v>
+      </c>
+    </row>
+    <row r="533" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A533" s="2" t="s">
+        <v>3770</v>
+      </c>
+    </row>
+    <row r="534" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A534" s="2" t="s">
+        <v>3771</v>
+      </c>
+    </row>
+    <row r="535" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A535" s="2" t="s">
+        <v>3772</v>
+      </c>
+    </row>
+    <row r="536" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A536" s="2" t="s">
+        <v>3773</v>
+      </c>
+    </row>
+    <row r="537" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A537" s="2" t="s">
+        <v>3774</v>
+      </c>
+    </row>
+    <row r="538" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A538" s="2" t="s">
+        <v>3775</v>
+      </c>
+    </row>
+    <row r="539" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A539" s="2" t="s">
+        <v>3776</v>
+      </c>
+    </row>
+    <row r="540" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A540" s="2" t="s">
+        <v>3777</v>
+      </c>
+    </row>
+    <row r="541" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A541" s="2" t="s">
+        <v>3778</v>
+      </c>
+    </row>
+    <row r="542" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A542" s="2" t="s">
+        <v>2700</v>
+      </c>
+      <c r="C542" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D542" s="2" t="s">
+        <v>2685</v>
+      </c>
+      <c r="E542" s="2" t="s">
+        <v>2696</v>
+      </c>
+      <c r="F542" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G542" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="H542" s="2" t="s">
+        <v>2697</v>
+      </c>
+      <c r="I542" s="2" t="s">
+        <v>2698</v>
+      </c>
+      <c r="K542" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L542" s="2" t="s">
+        <v>2699</v>
+      </c>
+      <c r="M542" s="2" t="s">
+        <v>2701</v>
+      </c>
+      <c r="O542" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="P542" s="2" t="s">
+        <v>2702</v>
+      </c>
+      <c r="Q542" s="2" t="s">
+        <v>2703</v>
+      </c>
+      <c r="R542" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="S542" s="2" t="s">
+        <v>2704</v>
+      </c>
+      <c r="T542" s="2" t="s">
+        <v>2705</v>
+      </c>
+      <c r="U542" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="V542" s="2" t="s">
+        <v>2706</v>
+      </c>
+      <c r="W542" s="2" t="s">
+        <v>2707</v>
+      </c>
+      <c r="X542" s="2" t="s">
+        <v>2708</v>
+      </c>
+      <c r="Y542" s="2" t="s">
+        <v>2700</v>
+      </c>
+      <c r="Z542" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA542" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="AB542" s="2" t="s">
+        <v>2597</v>
+      </c>
+      <c r="AC542" s="2" t="s">
+        <v>2701</v>
+      </c>
+      <c r="AD542" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="AE542" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="AF542" s="2" t="s">
+        <v>2702</v>
+      </c>
+    </row>
+    <row r="543" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A543" s="2" t="s">
+        <v>3779</v>
+      </c>
+    </row>
+    <row r="544" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A544" s="2" t="s">
+        <v>3780</v>
+      </c>
+    </row>
+    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A545" s="2" t="s">
+        <v>3781</v>
+      </c>
+    </row>
+    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A546" s="2" t="s">
+        <v>3782</v>
+      </c>
+    </row>
+    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A547" s="2" t="s">
+        <v>3783</v>
+      </c>
+    </row>
+    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A548" s="2" t="s">
+        <v>3784</v>
+      </c>
+    </row>
+    <row r="549" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A549" s="2" t="s">
+        <v>3785</v>
+      </c>
+    </row>
+    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A550" s="2" t="s">
+        <v>3786</v>
+      </c>
+    </row>
+    <row r="551" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A551" s="2" t="s">
+        <v>3787</v>
+      </c>
+    </row>
+    <row r="552" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A552" s="2" t="s">
+        <v>3788</v>
+      </c>
+    </row>
+    <row r="553" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A553" s="2" t="s">
+        <v>3789</v>
+      </c>
+    </row>
+    <row r="554" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A554" s="2" t="s">
+        <v>3790</v>
+      </c>
+    </row>
+    <row r="555" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A555" s="2" t="s">
+        <v>3791</v>
+      </c>
+    </row>
+    <row r="556" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A556" s="2" t="s">
+        <v>3792</v>
+      </c>
+    </row>
+    <row r="557" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A557" s="2" t="s">
+        <v>3793</v>
+      </c>
+    </row>
+    <row r="558" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A558" s="2" t="s">
+        <v>3794</v>
+      </c>
+    </row>
+    <row r="559" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A559" s="2" t="s">
+        <v>3795</v>
+      </c>
+    </row>
+    <row r="560" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A560" s="2" t="s">
+        <v>3796</v>
+      </c>
+    </row>
+    <row r="561" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A561" s="2" t="s">
+        <v>3797</v>
+      </c>
+    </row>
+    <row r="562" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A562" s="2" t="s">
+        <v>3798</v>
+      </c>
+    </row>
+    <row r="563" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A563" s="2" t="s">
+        <v>3799</v>
+      </c>
+    </row>
+    <row r="564" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A564" s="2" t="s">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="565" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A565" s="2" t="s">
+        <v>3801</v>
+      </c>
+    </row>
+    <row r="566" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A566" s="2" t="s">
+        <v>3802</v>
+      </c>
+    </row>
+    <row r="567" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A567" s="2" t="s">
+        <v>3803</v>
+      </c>
+    </row>
+    <row r="568" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A568" s="2" t="s">
+        <v>3804</v>
+      </c>
+    </row>
+    <row r="569" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A569" s="2" t="s">
+        <v>3805</v>
+      </c>
+    </row>
+    <row r="570" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A570" s="2" t="s">
+        <v>3806</v>
+      </c>
+    </row>
+    <row r="571" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A571" s="2" t="s">
+        <v>3807</v>
+      </c>
+    </row>
+    <row r="572" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A572" s="2" t="s">
+        <v>3808</v>
+      </c>
+    </row>
+    <row r="573" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A573" s="2" t="s">
+        <v>3809</v>
+      </c>
+    </row>
+    <row r="574" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A574" s="2" t="s">
+        <v>3810</v>
+      </c>
+    </row>
+    <row r="575" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A575" s="2" t="s">
+        <v>3811</v>
+      </c>
+    </row>
+    <row r="576" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A576" s="2" t="s">
+        <v>3812</v>
+      </c>
+    </row>
+    <row r="577" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A577" s="2" t="s">
+        <v>3813</v>
+      </c>
+    </row>
+    <row r="578" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A578" s="2" t="s">
+        <v>3814</v>
+      </c>
+    </row>
+    <row r="579" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A579" s="2" t="s">
+        <v>3815</v>
+      </c>
+    </row>
+    <row r="580" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A580" s="2" t="s">
+        <v>3816</v>
+      </c>
+    </row>
+    <row r="581" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A581" s="2" t="s">
+        <v>3817</v>
+      </c>
+    </row>
+    <row r="582" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A582" s="2" t="s">
+        <v>3818</v>
+      </c>
+    </row>
+    <row r="583" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A583" s="2" t="s">
+        <v>3819</v>
+      </c>
+    </row>
+    <row r="584" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A584" s="2" t="s">
+        <v>3820</v>
+      </c>
+    </row>
+    <row r="585" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A585" s="2" t="s">
+        <v>3821</v>
+      </c>
+    </row>
+    <row r="586" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A586" s="2" t="s">
+        <v>3822</v>
+      </c>
+    </row>
+    <row r="587" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A587" s="2" t="s">
+        <v>3823</v>
+      </c>
+    </row>
+    <row r="588" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A588" s="2" t="s">
+        <v>3824</v>
+      </c>
+    </row>
+    <row r="589" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A589" s="2" t="s">
+        <v>3825</v>
+      </c>
+    </row>
+    <row r="590" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A590" s="2" t="s">
+        <v>3826</v>
+      </c>
+    </row>
+    <row r="591" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A591" s="2" t="s">
+        <v>3827</v>
+      </c>
+    </row>
+    <row r="592" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A592" s="2" t="s">
+        <v>3828</v>
+      </c>
+    </row>
+    <row r="593" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A593" s="2" t="s">
+        <v>3829</v>
+      </c>
+    </row>
+    <row r="594" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A594" s="2" t="s">
+        <v>3830</v>
+      </c>
+    </row>
+    <row r="595" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A595" s="2" t="s">
+        <v>3831</v>
+      </c>
+    </row>
+    <row r="596" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A596" s="2" t="s">
+        <v>3832</v>
+      </c>
+    </row>
+    <row r="597" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A597" s="2" t="s">
+        <v>3833</v>
+      </c>
+    </row>
+    <row r="598" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A598" s="2" t="s">
+        <v>3834</v>
+      </c>
+    </row>
+    <row r="599" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A599" s="2" t="s">
+        <v>3835</v>
+      </c>
+    </row>
+    <row r="600" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A600" s="2" t="s">
+        <v>3836</v>
+      </c>
+    </row>
+    <row r="601" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A601" s="2" t="s">
+        <v>3837</v>
+      </c>
+    </row>
+    <row r="602" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A602" s="2" t="s">
+        <v>3838</v>
+      </c>
+    </row>
+    <row r="603" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A603" s="2" t="s">
+        <v>3839</v>
+      </c>
+    </row>
+    <row r="604" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A604" s="2" t="s">
+        <v>3840</v>
+      </c>
+    </row>
+    <row r="605" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A605" s="2" t="s">
+        <v>3841</v>
+      </c>
+    </row>
+    <row r="606" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A606" s="2" t="s">
+        <v>3842</v>
       </c>
     </row>
   </sheetData>

</xml_diff>